<commit_message>
Part 3 and 4, but kind of scuffed lol
</commit_message>
<xml_diff>
--- a/boundary/data/angle_data_formatted.xlsx
+++ b/boundary/data/angle_data_formatted.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jackson\physics_387\boundary\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCEF22FF-FE31-49C1-B976-5024EA1B2C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF409DF-D739-4C68-82C8-1EF2DFCCF8A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{951BB4D2-3E14-4958-B323-453993576732}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{951BB4D2-3E14-4958-B323-453993576732}"/>
   </bookViews>
   <sheets>
     <sheet name="Part1" sheetId="1" r:id="rId1"/>
@@ -719,7 +719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D052392-87C1-4C2D-9D4E-EDA12C4F9E29}">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
@@ -1380,10 +1380,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D7F469E-F1A7-472B-B94C-1D9B484914E1}">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1391,7 +1391,7 @@
     <col min="2" max="2" width="16.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1427,20 +1427,8 @@
       <c r="I2">
         <v>45</v>
       </c>
-      <c r="J2">
-        <v>40</v>
-      </c>
-      <c r="K2">
-        <v>30</v>
-      </c>
-      <c r="L2">
-        <v>20</v>
-      </c>
-      <c r="M2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C3">
         <v>180</v>
       </c>
@@ -1463,7 +1451,7 @@
         <v>153.5</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E4">
         <v>40</v>
       </c>
@@ -1479,20 +1467,8 @@
       <c r="I4">
         <v>90</v>
       </c>
-      <c r="J4">
-        <v>100.5</v>
-      </c>
-      <c r="K4">
-        <v>121</v>
-      </c>
-      <c r="L4">
-        <v>139</v>
-      </c>
-      <c r="M4">
-        <v>161.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5">
         <v>139</v>
       </c>
@@ -1515,7 +1491,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E6">
         <v>5.3</v>
       </c>
@@ -1531,20 +1507,8 @@
       <c r="I6">
         <v>122</v>
       </c>
-      <c r="J6">
-        <v>126</v>
-      </c>
-      <c r="K6">
-        <v>131</v>
-      </c>
-      <c r="L6">
-        <v>131</v>
-      </c>
-      <c r="M6">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1572,20 +1536,8 @@
       <c r="I7">
         <v>45</v>
       </c>
-      <c r="J7">
-        <v>40</v>
-      </c>
-      <c r="K7">
-        <v>30</v>
-      </c>
-      <c r="L7">
-        <v>20</v>
-      </c>
-      <c r="M7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>180</v>
       </c>
@@ -1608,7 +1560,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E9">
         <v>39</v>
       </c>
@@ -1624,20 +1576,8 @@
       <c r="I9">
         <v>89</v>
       </c>
-      <c r="J9">
-        <v>101</v>
-      </c>
-      <c r="K9">
-        <v>120</v>
-      </c>
-      <c r="L9">
-        <v>140.5</v>
-      </c>
-      <c r="M9">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C10">
         <v>73</v>
       </c>
@@ -1660,7 +1600,7 @@
         <v>0.13100000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E11">
         <v>1.97</v>
       </c>
@@ -1676,20 +1616,8 @@
       <c r="I11">
         <v>30.3</v>
       </c>
-      <c r="J11">
-        <v>28</v>
-      </c>
-      <c r="K11">
-        <v>31</v>
-      </c>
-      <c r="L11">
-        <v>30</v>
-      </c>
-      <c r="M11">
-        <v>33.799999999999997</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1720,17 +1648,8 @@
       <c r="J12">
         <v>40</v>
       </c>
-      <c r="K12">
-        <v>30</v>
-      </c>
-      <c r="L12">
-        <v>20</v>
-      </c>
-      <c r="M12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C13">
         <v>180</v>
       </c>
@@ -1756,7 +1675,7 @@
         <v>157.5</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E14">
         <v>42</v>
       </c>
@@ -1775,17 +1694,8 @@
       <c r="J14">
         <v>101.5</v>
       </c>
-      <c r="K14">
-        <v>119.5</v>
-      </c>
-      <c r="L14">
-        <v>140</v>
-      </c>
-      <c r="M14">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C15">
         <v>226</v>
       </c>
@@ -1811,7 +1721,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E16">
         <v>3.31</v>
       </c>
@@ -1830,17 +1740,8 @@
       <c r="J16">
         <v>168</v>
       </c>
-      <c r="K16">
-        <v>182</v>
-      </c>
-      <c r="L16">
-        <v>200</v>
-      </c>
-      <c r="M16">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -1871,17 +1772,8 @@
       <c r="J17">
         <v>40</v>
       </c>
-      <c r="K17">
-        <v>30</v>
-      </c>
-      <c r="L17">
-        <v>20</v>
-      </c>
-      <c r="M17">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C18">
         <v>180</v>
       </c>
@@ -1906,17 +1798,8 @@
       <c r="J18">
         <v>180</v>
       </c>
-      <c r="K18">
-        <v>180</v>
-      </c>
-      <c r="L18">
-        <v>180</v>
-      </c>
-      <c r="M18">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E19">
         <v>36.5</v>
       </c>
@@ -1935,17 +1818,8 @@
       <c r="J19">
         <v>98.5</v>
       </c>
-      <c r="K19">
-        <v>120</v>
-      </c>
-      <c r="L19">
-        <v>140</v>
-      </c>
-      <c r="M19">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C20">
         <v>113</v>
       </c>
@@ -1970,17 +1844,8 @@
       <c r="J20">
         <v>2.17</v>
       </c>
-      <c r="K20">
-        <v>2.17</v>
-      </c>
-      <c r="L20">
-        <v>2</v>
-      </c>
-      <c r="M20">
-        <v>3.2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E21">
         <v>1</v>
       </c>
@@ -1998,15 +1863,6 @@
       </c>
       <c r="J21">
         <v>36.5</v>
-      </c>
-      <c r="K21">
-        <v>37</v>
-      </c>
-      <c r="L21">
-        <v>40.299999999999997</v>
-      </c>
-      <c r="M21">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>